<commit_message>
Generate Group Marking Form
</commit_message>
<xml_diff>
--- a/IT114115_FYP_MarkSheet_Template.xlsx
+++ b/IT114115_FYP_MarkSheet_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyrus\Desktop\FYP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\IVE\Course\NHD Project\1516\Marksheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="117">
   <si>
     <t>Weighting</t>
   </si>
@@ -310,9 +310,6 @@
     <t>Overall (0-30):</t>
   </si>
   <si>
-    <t>B2</t>
-  </si>
-  <si>
     <t>Cyrus Wong</t>
   </si>
   <si>
@@ -434,9 +431,6 @@
   </si>
   <si>
     <t>YYYY</t>
-  </si>
-  <si>
-    <t>IT114115/2X</t>
   </si>
 </sst>
 </file>
@@ -1845,7 +1839,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1863,8 +1857,9 @@
       <c r="A1" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="106" t="s">
-        <v>118</v>
+      <c r="B1" s="106" t="str">
+        <f>"IT114115/2"&amp;LEFT( B3, 1)</f>
+        <v>IT114115/2</v>
       </c>
       <c r="C1" s="70"/>
       <c r="D1" s="70"/>
@@ -1880,7 +1875,7 @@
       <c r="B2" s="107"/>
       <c r="C2" s="70"/>
       <c r="D2" s="70" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E2" s="70">
         <f>COUNTA(B5:B8)</f>
@@ -1894,35 +1889,33 @@
       <c r="A3" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="106" t="s">
-        <v>82</v>
-      </c>
+      <c r="B3" s="106"/>
       <c r="C3" s="70"/>
       <c r="D3" s="116" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="116" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" s="116" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" s="116" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="116" t="s">
-        <v>110</v>
-      </c>
-      <c r="F3" s="116" t="s">
-        <v>111</v>
-      </c>
-      <c r="G3" s="116" t="s">
-        <v>94</v>
-      </c>
       <c r="H3" s="117" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75">
       <c r="A4" s="108" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="109" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="109" t="s">
+      <c r="C4" s="108" t="s">
         <v>106</v>
-      </c>
-      <c r="C4" s="108" t="s">
-        <v>107</v>
       </c>
       <c r="D4" s="105">
         <v>0.1</v>
@@ -1945,7 +1938,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="111" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" s="108">
         <v>123456688</v>
@@ -1976,7 +1969,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="111" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6" s="108">
         <v>123456789</v>
@@ -2071,10 +2064,10 @@
         <v>47</v>
       </c>
       <c r="B10" s="114" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" s="70" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D10" s="113">
         <v>41992</v>
@@ -2086,13 +2079,13 @@
     </row>
     <row r="11" spans="1:9" ht="15">
       <c r="A11" s="112" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" s="114" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D11" s="113">
         <v>42017</v>
@@ -2104,13 +2097,13 @@
     </row>
     <row r="12" spans="1:9" ht="15">
       <c r="A12" s="112" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="114" t="s">
         <v>99</v>
       </c>
-      <c r="B12" s="114" t="s">
-        <v>100</v>
-      </c>
       <c r="C12" s="70" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D12" s="113">
         <v>42123</v>
@@ -2122,7 +2115,7 @@
     </row>
     <row r="15" spans="1:9" ht="15.75">
       <c r="A15" s="118" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75">
@@ -2668,7 +2661,7 @@
     </row>
     <row r="46" spans="1:9" ht="15.75">
       <c r="A46" s="126" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="18.75">
@@ -3460,7 +3453,7 @@
     </row>
     <row r="93" spans="1:9" ht="15.75">
       <c r="A93" s="126" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="18.75">
@@ -3595,7 +3588,7 @@
         <v/>
       </c>
       <c r="D102" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E102" s="23" t="s">
         <v>21</v>
@@ -3951,7 +3944,7 @@
     <row r="3" spans="1:10" ht="15.75">
       <c r="A3" s="3"/>
       <c r="B3" s="152" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="152"/>
       <c r="D3" s="152"/>
@@ -3981,7 +3974,7 @@
       </c>
       <c r="C5" s="4" t="str">
         <f>'Project Summary'!B1</f>
-        <v>IT114115/2X</v>
+        <v>IT114115/2</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
@@ -4020,9 +4013,9 @@
       <c r="B7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="98" t="str">
+      <c r="C7" s="98">
         <f>'Project Summary'!B3</f>
-        <v>B2</v>
+        <v>0</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
@@ -4572,16 +4565,16 @@
       </c>
       <c r="C4" s="50" t="str">
         <f>'Project Summary'!B1</f>
-        <v>IT114115/2X</v>
+        <v>IT114115/2</v>
       </c>
       <c r="D4" s="49"/>
       <c r="E4" s="51" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="49"/>
-      <c r="G4" s="165" t="str">
+      <c r="G4" s="165">
         <f>'Project Summary'!B3</f>
-        <v>B2</v>
+        <v>0</v>
       </c>
       <c r="H4" s="165"/>
       <c r="I4" s="165"/>
@@ -5265,7 +5258,7 @@
     </row>
     <row r="2" spans="1:9" s="48" customFormat="1" ht="20.25">
       <c r="A2" s="164" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="164"/>
       <c r="C2" s="164"/>
@@ -5294,16 +5287,16 @@
       </c>
       <c r="C4" s="101" t="str">
         <f>'Project Summary'!B1</f>
-        <v>IT114115/2X</v>
+        <v>IT114115/2</v>
       </c>
       <c r="D4" s="49"/>
       <c r="E4" s="51" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="49"/>
-      <c r="G4" s="165" t="str">
+      <c r="G4" s="165">
         <f>'Project Summary'!B3</f>
-        <v>B2</v>
+        <v>0</v>
       </c>
       <c r="H4" s="165"/>
       <c r="I4" s="165"/>
@@ -6018,7 +6011,7 @@
       </c>
       <c r="C4" s="50" t="str">
         <f>'Project Summary'!B1</f>
-        <v>IT114115/2X</v>
+        <v>IT114115/2</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="148" t="s">
@@ -6037,9 +6030,9 @@
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="104" t="str">
+      <c r="C5" s="104">
         <f>'Project Summary'!B3</f>
-        <v>B2</v>
+        <v>0</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="148" t="s">
@@ -7101,7 +7094,7 @@
     </row>
     <row r="2" spans="1:9" s="7" customFormat="1" ht="20.25">
       <c r="A2" s="167" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="167"/>
       <c r="C2" s="167"/>
@@ -7130,7 +7123,7 @@
       </c>
       <c r="C4" s="103" t="str">
         <f>'Project Summary'!B1</f>
-        <v>IT114115/2X</v>
+        <v>IT114115/2</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="148" t="s">
@@ -7149,9 +7142,9 @@
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="104" t="str">
+      <c r="C5" s="104">
         <f>'Project Summary'!B3</f>
-        <v>B2</v>
+        <v>0</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="148" t="s">
@@ -8154,7 +8147,7 @@
     </row>
     <row r="2" spans="1:14" s="70" customFormat="1" ht="15.75">
       <c r="A2" s="69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="172" t="str">
         <f>'Project Summary'!B10</f>
@@ -8175,7 +8168,7 @@
     </row>
     <row r="3" spans="1:14" s="70" customFormat="1" ht="15.75">
       <c r="A3" s="71" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="172" t="str">
         <f>'Project Summary'!B11&amp;"(Semester 1) /  "&amp;'Project Summary'!B12&amp;"(Semester 2)"</f>
@@ -8196,7 +8189,7 @@
     </row>
     <row r="4" spans="1:14" s="70" customFormat="1" ht="73.150000000000006" customHeight="1">
       <c r="A4" s="72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="173"/>
       <c r="C4" s="172"/>
@@ -8232,19 +8225,19 @@
       <c r="A6" s="73"/>
       <c r="B6" s="73"/>
       <c r="C6" s="174" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" s="174"/>
       <c r="E6" s="174"/>
       <c r="F6" s="174"/>
       <c r="G6" s="175" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H6" s="175"/>
       <c r="I6" s="175"/>
       <c r="J6" s="175"/>
       <c r="K6" s="176" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L6" s="176"/>
       <c r="M6" s="176"/>
@@ -8252,25 +8245,25 @@
     </row>
     <row r="7" spans="1:14" s="70" customFormat="1" ht="15.75">
       <c r="A7" s="177" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="178" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="178" t="s">
+      <c r="C7" s="179" t="s">
         <v>91</v>
-      </c>
-      <c r="C7" s="179" t="s">
-        <v>92</v>
       </c>
       <c r="D7" s="179"/>
       <c r="E7" s="179"/>
       <c r="F7" s="179"/>
       <c r="G7" s="179" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H7" s="179"/>
       <c r="I7" s="179"/>
       <c r="J7" s="179"/>
       <c r="K7" s="179" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L7" s="179"/>
       <c r="M7" s="179"/>
@@ -8318,7 +8311,7 @@
     </row>
     <row r="9" spans="1:14" s="70" customFormat="1" ht="15.75">
       <c r="A9" s="75" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" s="76">
         <v>0.1</v>
@@ -8362,7 +8355,7 @@
     </row>
     <row r="10" spans="1:14" s="70" customFormat="1" ht="47.25">
       <c r="A10" s="80" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" s="76">
         <v>0.3</v>
@@ -8418,7 +8411,7 @@
     </row>
     <row r="11" spans="1:14" s="70" customFormat="1" ht="47.25">
       <c r="A11" s="80" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B11" s="76">
         <v>0.5</v>
@@ -8474,7 +8467,7 @@
     </row>
     <row r="12" spans="1:14" s="70" customFormat="1" ht="15.75">
       <c r="A12" s="75" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="76">
         <v>0.1</v>
@@ -8518,7 +8511,7 @@
     </row>
     <row r="13" spans="1:14" s="86" customFormat="1" ht="16.5" thickBot="1">
       <c r="A13" s="81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="82">
         <f>SUM(B9:B12)</f>

</xml_diff>